<commit_message>
Format, streamline analysis, order work
also changed traits back to day, not effect size
</commit_message>
<xml_diff>
--- a/analyses/Results from stan models 2016-03-30.xlsx
+++ b/analyses/Results from stan models 2016-03-30.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="720" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="16300" yWindow="880" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>n_eff</t>
   </si>
@@ -58,6 +58,33 @@
   </si>
   <si>
     <t xml:space="preserve">leafout </t>
+  </si>
+  <si>
+    <t>mu_b_site</t>
+  </si>
+  <si>
+    <t>mu_b_inter_wp</t>
+  </si>
+  <si>
+    <t>mu_b_inter_ws</t>
+  </si>
+  <si>
+    <t>mu_b_inter_ps</t>
+  </si>
+  <si>
+    <t>mu_b_inter_wc1</t>
+  </si>
+  <si>
+    <t>mu_b_inter_wc2</t>
+  </si>
+  <si>
+    <t>lday_site_sp_chill_inter</t>
+  </si>
+  <si>
+    <t>chilling as two levels, with interactions</t>
+  </si>
+  <si>
+    <t>leafout</t>
   </si>
 </sst>
 </file>
@@ -452,15 +479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -831,6 +858,401 @@
       </c>
       <c r="K16">
         <v>-5.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>236</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>-21.9</v>
+      </c>
+      <c r="E22">
+        <v>0.1</v>
+      </c>
+      <c r="F22">
+        <v>1.7</v>
+      </c>
+      <c r="G22">
+        <v>-25.3</v>
+      </c>
+      <c r="H22">
+        <v>-23</v>
+      </c>
+      <c r="I22">
+        <v>-21.9</v>
+      </c>
+      <c r="J22">
+        <v>-20.7</v>
+      </c>
+      <c r="K22">
+        <v>-18.600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>475</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>-26.4</v>
+      </c>
+      <c r="E23">
+        <v>0.1</v>
+      </c>
+      <c r="F23">
+        <v>3.1</v>
+      </c>
+      <c r="G23">
+        <v>-32.4</v>
+      </c>
+      <c r="H23">
+        <v>-28.4</v>
+      </c>
+      <c r="I23">
+        <v>-26.4</v>
+      </c>
+      <c r="J23">
+        <v>-24.4</v>
+      </c>
+      <c r="K23">
+        <v>-20.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>345</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>-26.1</v>
+      </c>
+      <c r="E24">
+        <v>0.2</v>
+      </c>
+      <c r="F24">
+        <v>3.1</v>
+      </c>
+      <c r="G24">
+        <v>-32.1</v>
+      </c>
+      <c r="H24">
+        <v>-28.3</v>
+      </c>
+      <c r="I24">
+        <v>-26.2</v>
+      </c>
+      <c r="J24">
+        <v>-24</v>
+      </c>
+      <c r="K24">
+        <v>-20.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>270</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>-13.7</v>
+      </c>
+      <c r="E25">
+        <v>0.1</v>
+      </c>
+      <c r="F25">
+        <v>1.7</v>
+      </c>
+      <c r="G25">
+        <v>-17</v>
+      </c>
+      <c r="H25">
+        <v>-14.8</v>
+      </c>
+      <c r="I25">
+        <v>-13.7</v>
+      </c>
+      <c r="J25">
+        <v>-12.6</v>
+      </c>
+      <c r="K25">
+        <v>-10.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>214</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0.1</v>
+      </c>
+      <c r="F26">
+        <v>2.1</v>
+      </c>
+      <c r="G26">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H26">
+        <v>1.7</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K26">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>320</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>3.5</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0.8</v>
+      </c>
+      <c r="G27">
+        <v>2.1</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>3.5</v>
+      </c>
+      <c r="J27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K27">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>141</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>-0.6</v>
+      </c>
+      <c r="E28">
+        <v>0.1</v>
+      </c>
+      <c r="F28">
+        <v>0.8</v>
+      </c>
+      <c r="G28">
+        <v>-2.4</v>
+      </c>
+      <c r="H28">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="I28">
+        <v>-0.6</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>217</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>0.1</v>
+      </c>
+      <c r="F29">
+        <v>0.8</v>
+      </c>
+      <c r="G29">
+        <v>-2.6</v>
+      </c>
+      <c r="H29">
+        <v>-1.6</v>
+      </c>
+      <c r="I29">
+        <v>-1</v>
+      </c>
+      <c r="J29">
+        <v>-0.4</v>
+      </c>
+      <c r="K29">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <v>769</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1.2</v>
+      </c>
+      <c r="G30">
+        <v>7.8</v>
+      </c>
+      <c r="H30">
+        <v>9.5</v>
+      </c>
+      <c r="I30">
+        <v>10.1</v>
+      </c>
+      <c r="J30">
+        <v>10.9</v>
+      </c>
+      <c r="K30">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31">
+        <v>224</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>11.3</v>
+      </c>
+      <c r="E31">
+        <v>0.1</v>
+      </c>
+      <c r="F31">
+        <v>1.2</v>
+      </c>
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>10.4</v>
+      </c>
+      <c r="I31">
+        <v>11.3</v>
+      </c>
+      <c r="J31">
+        <v>12.1</v>
+      </c>
+      <c r="K31">
+        <v>13.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>